<commit_message>
Update for readability & remove unnecessary code
</commit_message>
<xml_diff>
--- a/snakeData.xlsx
+++ b/snakeData.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcarter11\Downloads\_Spring2024\CS461\FinalProject\__FinalProjectCodes\dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcarter11\Downloads\_Fall2024\zProjects\zother\SnakeClassificationSystem\SnakeSpeciesClassification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890E4DB8-2683-4A36-A69C-4CD3D27FE0A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18294020-C408-4C5F-B9F6-2B8BFEBC089C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{8E74549D-7FC8-4161-ADCC-A28EA14143B5}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" xr2:uid="{8E74549D-7FC8-4161-ADCC-A28EA14143B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Classification" sheetId="1" r:id="rId1"/>
     <sheet name="TrainingData" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1580" uniqueCount="42">
   <si>
     <t>slender</t>
   </si>
@@ -157,6 +158,12 @@
   </si>
   <si>
     <t>ScaleTexture</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>venomous</t>
   </si>
 </sst>
 </file>
@@ -536,14 +543,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{381940C2-C9F5-4CC4-B3A3-A5016DDD50AF}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -552,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E229DEB1-62FD-44F7-B661-5B44BBE5C48C}">
   <dimension ref="A1:N116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I71" sqref="I71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1471,25 +1571,25 @@
     </row>
     <row r="32" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
@@ -1516,10 +1616,10 @@
         <v>19</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -1534,7 +1634,7 @@
         <v>20</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>18</v>
@@ -1546,10 +1646,10 @@
         <v>19</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
@@ -1564,7 +1664,7 @@
         <v>20</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>18</v>
@@ -1669,7 +1769,7 @@
         <v>4</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
@@ -1684,7 +1784,7 @@
         <v>20</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>18</v>
@@ -1699,7 +1799,7 @@
         <v>4</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
@@ -1714,7 +1814,7 @@
         <v>20</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>18</v>
@@ -1771,22 +1871,22 @@
     </row>
     <row r="42" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>1</v>
@@ -1807,7 +1907,7 @@
         <v>17</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>21</v>
@@ -1834,10 +1934,10 @@
         <v>24</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>21</v>
@@ -1849,7 +1949,7 @@
         <v>23</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
@@ -1864,7 +1964,7 @@
         <v>24</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>1</v>
@@ -1879,7 +1979,7 @@
         <v>23</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -1894,7 +1994,7 @@
         <v>24</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>1</v>
@@ -1924,7 +2024,7 @@
         <v>24</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>1</v>
@@ -1939,7 +2039,7 @@
         <v>23</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
@@ -1969,7 +2069,7 @@
         <v>23</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
@@ -2017,7 +2117,7 @@
         <v>17</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>21</v>
@@ -2044,10 +2144,10 @@
         <v>24</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>21</v>
@@ -2071,22 +2171,22 @@
     </row>
     <row r="52" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>1</v>
@@ -2101,22 +2201,22 @@
     </row>
     <row r="53" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>1</v>
@@ -2209,7 +2309,7 @@
         <v>4</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
@@ -2239,7 +2339,7 @@
         <v>4</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
@@ -2269,7 +2369,7 @@
         <v>4</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
@@ -2299,7 +2399,7 @@
         <v>4</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
@@ -2329,7 +2429,7 @@
         <v>4</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
@@ -2371,13 +2471,13 @@
     </row>
     <row r="62" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>14</v>
@@ -2389,7 +2489,7 @@
         <v>4</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
@@ -2401,13 +2501,13 @@
     </row>
     <row r="63" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>14</v>
@@ -2419,7 +2519,7 @@
         <v>4</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
@@ -2479,7 +2579,7 @@
         <v>4</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
@@ -2509,7 +2609,7 @@
         <v>4</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
@@ -2614,7 +2714,7 @@
         <v>27</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>1</v>
@@ -2629,7 +2729,7 @@
         <v>4</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
@@ -2659,7 +2759,7 @@
         <v>4</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
@@ -2671,22 +2771,22 @@
     </row>
     <row r="72" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>12</v>
@@ -2701,22 +2801,22 @@
     </row>
     <row r="73" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>6</v>
@@ -2734,7 +2834,7 @@
         <v>28</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>25</v>
@@ -2749,7 +2849,7 @@
         <v>11</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
@@ -2764,7 +2864,7 @@
         <v>28</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>25</v>
@@ -2779,7 +2879,7 @@
         <v>11</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
@@ -2794,7 +2894,7 @@
         <v>28</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>25</v>
@@ -2824,7 +2924,7 @@
         <v>28</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>25</v>
@@ -2899,7 +2999,7 @@
         <v>11</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
@@ -2959,7 +3059,7 @@
         <v>11</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
@@ -2971,7 +3071,7 @@
     </row>
     <row r="82" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>7</v>
@@ -2980,7 +3080,7 @@
         <v>25</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>19</v>
@@ -2989,7 +3089,7 @@
         <v>11</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
@@ -3001,7 +3101,7 @@
     </row>
     <row r="83" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>7</v>
@@ -3010,7 +3110,7 @@
         <v>25</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>19</v>
@@ -3169,7 +3269,7 @@
         <v>11</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
@@ -3196,10 +3296,10 @@
         <v>19</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
@@ -3229,7 +3329,7 @@
         <v>11</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
@@ -3256,7 +3356,7 @@
         <v>19</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>6</v>
@@ -3271,25 +3371,25 @@
     </row>
     <row r="92" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
@@ -3301,25 +3401,25 @@
     </row>
     <row r="93" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H93" s="1"/>
       <c r="I93" s="1"/>
@@ -3424,7 +3524,7 @@
         <v>30</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>1</v>
@@ -3433,7 +3533,7 @@
         <v>14</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>4</v>
@@ -3484,7 +3584,7 @@
         <v>30</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>1</v>
@@ -3493,7 +3593,7 @@
         <v>14</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>4</v>
@@ -3514,7 +3614,7 @@
         <v>30</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>1</v>
@@ -3571,25 +3671,25 @@
     </row>
     <row r="102" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H102" s="1"/>
       <c r="I102" s="1"/>
@@ -3601,7 +3701,7 @@
     </row>
     <row r="103" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>0</v>
@@ -3610,10 +3710,10 @@
         <v>1</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>4</v>
@@ -3637,10 +3737,10 @@
         <v>17</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>3</v>
@@ -3664,10 +3764,10 @@
         <v>31</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>2</v>
@@ -3700,13 +3800,13 @@
         <v>25</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="G106" s="1" t="s">
         <v>6</v>
@@ -3730,10 +3830,10 @@
         <v>18</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>4</v>
@@ -3757,16 +3857,16 @@
         <v>17</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="G108" s="1" t="s">
         <v>6</v>
@@ -3784,22 +3884,22 @@
         <v>31</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H109" s="1"/>
       <c r="I109" s="1"/>
@@ -3814,10 +3914,10 @@
         <v>31</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>9</v>
@@ -3826,7 +3926,7 @@
         <v>19</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G110" s="1" t="s">
         <v>6</v>
@@ -3844,22 +3944,22 @@
         <v>31</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H111" s="1"/>
       <c r="I111" s="1"/>
@@ -3870,27 +3970,6 @@
       <c r="N111" s="1"/>
     </row>
     <row r="112" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F112" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G112" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="H112" s="1"/>
       <c r="I112" s="1"/>
       <c r="J112" s="1"/>
@@ -3899,28 +3978,7 @@
       <c r="M112" s="1"/>
       <c r="N112" s="1"/>
     </row>
-    <row r="113" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E113" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F113" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G113" s="1" t="s">
-        <v>6</v>
-      </c>
+    <row r="113" spans="8:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H113" s="1"/>
       <c r="I113" s="1"/>
       <c r="J113" s="1"/>
@@ -3929,7 +3987,7 @@
       <c r="M113" s="1"/>
       <c r="N113" s="1"/>
     </row>
-    <row r="114" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="114" spans="8:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H114" s="1"/>
       <c r="I114" s="1"/>
       <c r="J114" s="1"/>
@@ -3938,7 +3996,7 @@
       <c r="M114" s="1"/>
       <c r="N114" s="1"/>
     </row>
-    <row r="115" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="8:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H115" s="1"/>
       <c r="I115" s="1"/>
       <c r="J115" s="1"/>
@@ -3947,7 +4005,7 @@
       <c r="M115" s="1"/>
       <c r="N115" s="1"/>
     </row>
-    <row r="116" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="116" spans="8:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H116" s="1"/>
       <c r="I116" s="1"/>
       <c r="J116" s="1"/>
@@ -3959,4 +4017,2627 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{487309C4-029F-437C-9EAA-2FD64AA78870}">
+  <dimension ref="A1:G113"/>
+  <sheetViews>
+    <sheetView topLeftCell="A93" workbookViewId="0">
+      <selection sqref="A1:G113"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>